<commit_message>
Updating Ch 2 mostly
</commit_message>
<xml_diff>
--- a/chapterFiles/rdmReview/methodsOverview.xlsx
+++ b/chapterFiles/rdmReview/methodsOverview.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaburnett/Documents/GitHub/myDissertation/chapterFiles/rdmReview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\myDissertation\chapterFiles\rdmReview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F13CBF-2C5B-3E41-B92B-32919A3757E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="26880" windowHeight="17544" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="rawListMethods" sheetId="1" r:id="rId1"/>
     <sheet name="methodsSummary" sheetId="2" r:id="rId2"/>
-    <sheet name="reviews" sheetId="3" r:id="rId3"/>
+    <sheet name="reviewPapers" sheetId="3" r:id="rId3"/>
+    <sheet name="usingManyIndicators" sheetId="4" r:id="rId4"/>
+    <sheet name="metaAnalysis" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="abstract0" localSheetId="2">reviews!$A$41</definedName>
-    <definedName name="article1.body1.sec1.p1" localSheetId="2">reviews!$A$73</definedName>
-    <definedName name="article1.body1.sec1.p2" localSheetId="2">reviews!$A$74</definedName>
-    <definedName name="article1.body1.sec1.p3" localSheetId="2">reviews!$A$87</definedName>
+    <definedName name="abstract0" localSheetId="2">reviewPapers!$A$41</definedName>
+    <definedName name="article1.body1.sec1.p1" localSheetId="2">reviewPapers!$A$73</definedName>
+    <definedName name="article1.body1.sec1.p2" localSheetId="2">reviewPapers!$A$74</definedName>
+    <definedName name="article1.body1.sec1.p3" localSheetId="2">reviewPapers!$A$87</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="229">
   <si>
     <t>Autocorrelation at-lag-1</t>
   </si>
@@ -509,9 +510,6 @@
     <t>method</t>
   </si>
   <si>
-    <t>Power spectral analysis</t>
-  </si>
-  <si>
     <t>return rate</t>
   </si>
   <si>
@@ -524,9 +522,6 @@
     <t>autoregressive model</t>
   </si>
   <si>
-    <t xml:space="preserve">from Dakos 2012: </t>
-  </si>
-  <si>
     <t>DFA fluctuation exponent</t>
   </si>
   <si>
@@ -635,14 +630,104 @@
     <t>-</t>
   </si>
   <si>
-    <t>simiulated</t>
+    <t>Fourier coefficients</t>
+  </si>
+  <si>
+    <t>lindegren2012early</t>
+  </si>
+  <si>
+    <t>AR1</t>
+  </si>
+  <si>
+    <t>Spectral analysis</t>
+  </si>
+  <si>
+    <t>GAM</t>
+  </si>
+  <si>
+    <t>Moran's I autocorrelation</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Alertogram</t>
+  </si>
+  <si>
+    <t>Shiftogram</t>
+  </si>
+  <si>
+    <t>empirical</t>
+  </si>
+  <si>
+    <t>signals on detrended data</t>
+  </si>
+  <si>
+    <t>boettiger2010regime</t>
+  </si>
+  <si>
+    <t>prosecutor's fallacy</t>
+  </si>
+  <si>
+    <t>sommer2017generic</t>
+  </si>
+  <si>
+    <t>perretti2012regime</t>
+  </si>
+  <si>
+    <t>effect of low, med and high noise on EWIs</t>
+  </si>
+  <si>
+    <t>ar1</t>
+  </si>
+  <si>
+    <t>"+ when low noise and high data points"</t>
+  </si>
+  <si>
+    <t>hare_empirical_2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papers that use multiple indicators but are just doing case studies and not </t>
+  </si>
+  <si>
+    <t>contamin2009indicators</t>
+  </si>
+  <si>
+    <t>empirical data</t>
+  </si>
+  <si>
+    <t>dutta2018robustness</t>
+  </si>
+  <si>
+    <t>dakos2012robustness</t>
+  </si>
+  <si>
+    <t>effect of various decisions reuqired by the data analyst on the results</t>
+  </si>
+  <si>
+    <t>"+ in saddle node, - in other"</t>
+  </si>
+  <si>
+    <t>varying variance of system prior to transition</t>
+  </si>
+  <si>
+    <t>litzow_early_2016</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>Reviewed published studies to determine what types of transitions should be expected in empirical systems dynamics. Also tested multiple ewis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +778,14 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -714,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -736,6 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,22 +1109,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C43" sqref="C43:D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="2"/>
+    <col min="1" max="2" width="8.77734375" style="2"/>
     <col min="3" max="9" width="37" style="1" customWidth="1"/>
     <col min="10" max="12" width="37" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="2"/>
+    <col min="13" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>122</v>
       </c>
@@ -1059,7 +1153,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1167,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1179,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1196,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1113,7 +1207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>105</v>
       </c>
@@ -1127,7 +1221,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>104</v>
       </c>
@@ -1141,7 +1235,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1152,16 +1246,16 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>124</v>
       </c>
@@ -1172,7 +1266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1180,7 +1274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1196,7 +1290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1204,7 +1298,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1212,7 +1306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1220,7 +1314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1228,7 +1322,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1330,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1244,7 +1338,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1252,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
@@ -1260,7 +1354,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1268,7 +1362,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1276,7 +1370,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>37</v>
       </c>
@@ -1284,7 +1378,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1292,7 +1386,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
@@ -1300,7 +1394,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>43</v>
       </c>
@@ -1308,7 +1402,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
         <v>45</v>
       </c>
@@ -1316,12 +1410,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>48</v>
       </c>
@@ -1329,7 +1423,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>50</v>
       </c>
@@ -1337,12 +1431,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="3:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>117</v>
       </c>
@@ -1350,7 +1444,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1358,7 +1452,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>55</v>
       </c>
@@ -1366,7 +1460,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
         <v>57</v>
       </c>
@@ -1374,7 +1468,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
         <v>58</v>
       </c>
@@ -1382,12 +1476,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
         <v>61</v>
       </c>
@@ -1395,7 +1489,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" s="7" t="s">
         <v>63</v>
       </c>
@@ -1403,7 +1497,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1411,7 +1505,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" s="1" t="s">
         <v>67</v>
       </c>
@@ -1419,7 +1513,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="3:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
         <v>69</v>
       </c>
@@ -1427,7 +1521,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="3:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
         <v>71</v>
       </c>
@@ -1435,7 +1529,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C48" s="1" t="s">
         <v>73</v>
       </c>
@@ -1443,7 +1537,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="3:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
         <v>75</v>
       </c>
@@ -1451,7 +1545,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="1" t="s">
         <v>77</v>
       </c>
@@ -1459,17 +1553,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C51" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="3:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
         <v>81</v>
       </c>
@@ -1477,7 +1571,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" s="1" t="s">
         <v>83</v>
       </c>
@@ -1485,7 +1579,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
         <v>85</v>
       </c>
@@ -1493,7 +1587,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C56" s="1" t="s">
         <v>87</v>
       </c>
@@ -1501,7 +1595,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="1" t="s">
         <v>89</v>
       </c>
@@ -1509,7 +1603,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="3:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C58" s="1" t="s">
         <v>91</v>
       </c>
@@ -1517,7 +1611,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="1" t="s">
         <v>92</v>
       </c>
@@ -1525,7 +1619,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C60" s="1" t="s">
         <v>94</v>
       </c>
@@ -1533,7 +1627,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="1" t="s">
         <v>96</v>
       </c>
@@ -1541,7 +1635,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" s="1" t="s">
         <v>97</v>
       </c>
@@ -1549,12 +1643,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="3:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C63" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" s="1" t="s">
         <v>100</v>
       </c>
@@ -1562,7 +1656,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="1" t="s">
         <v>102</v>
       </c>
@@ -1576,25 +1670,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ED7290-C50A-3146-A093-3439CA4E156D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="23.33203125" style="5" customWidth="1"/>
-    <col min="3" max="4" width="34.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="5"/>
-    <col min="6" max="6" width="9.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="5" customWidth="1"/>
+    <col min="3" max="4" width="34.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="5"/>
+    <col min="6" max="6" width="9.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="19" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="5"/>
+    <col min="9" max="16384" width="10.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>134</v>
       </c>
@@ -1617,7 +1711,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>135</v>
       </c>
@@ -1640,7 +1734,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>135</v>
       </c>
@@ -1663,7 +1757,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>135</v>
       </c>
@@ -1686,7 +1780,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>64</v>
       </c>
@@ -1709,7 +1803,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -1732,7 +1826,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>103</v>
       </c>
@@ -1740,7 +1834,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
@@ -1750,29 +1844,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E585EB-BD00-C342-9B39-195241830C95}">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="11" width="10.83203125" style="10"/>
+    <col min="1" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="11" width="10.77734375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>134</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>127</v>
@@ -1784,7 +1880,7 @@
         <v>123</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>130</v>
@@ -1796,24 +1892,24 @@
         <v>156</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
         <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
         <v>154</v>
@@ -1822,190 +1918,190 @@
         <v>141</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
         <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
         <v>128</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="F4" t="s">
         <v>155</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
         <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>141</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
         <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J6" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="K6" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
         <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J7" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s">
         <v>128</v>
@@ -2020,24 +2116,24 @@
         <v>139</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J8" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
         <v>128</v>
@@ -2046,97 +2142,97 @@
         <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
         <v>128</v>
       </c>
       <c r="D10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F10" t="s">
         <v>172</v>
       </c>
-      <c r="E10" t="s">
-        <v>175</v>
-      </c>
-      <c r="F10" t="s">
-        <v>174</v>
-      </c>
       <c r="G10" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
         <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>141</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
         <v>128</v>
@@ -2145,68 +2241,68 @@
         <v>138</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D13" t="s">
         <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>141</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D14" t="s">
         <v>153</v>
@@ -2215,33 +2311,33 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>141</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
         <v>153</v>
@@ -2250,33 +2346,33 @@
         <v>22</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C16" t="s">
         <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
         <v>129</v>
@@ -2285,55 +2381,690 @@
         <v>129</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J16" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
         <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" t="s">
+        <v>201</v>
+      </c>
+      <c r="F21" t="s">
         <v>198</v>
       </c>
-      <c r="F17" t="s">
-        <v>198</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="G21" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" t="s">
+        <v>200</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>199</v>
+      </c>
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" t="s">
+        <v>202</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" t="s">
+        <v>204</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>199</v>
+      </c>
+      <c r="B28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E28" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>209</v>
+      </c>
+      <c r="B29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29" t="s">
+        <v>200</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>211</v>
+      </c>
+      <c r="E31" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" t="s">
+        <v>158</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E34" t="s">
+        <v>139</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>211</v>
+      </c>
+      <c r="E35" t="s">
+        <v>169</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>212</v>
+      </c>
+      <c r="B36" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" t="s">
+        <v>214</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="E38" t="s">
+        <v>201</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" t="s">
+        <v>213</v>
+      </c>
+      <c r="E39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40" t="s">
+        <v>213</v>
+      </c>
+      <c r="E40" t="s">
+        <v>169</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>220</v>
+      </c>
+      <c r="B41" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" t="s">
+        <v>129</v>
+      </c>
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>163</v>
+      <c r="F42" t="s">
+        <v>214</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>224</v>
+      </c>
+      <c r="E43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" t="s">
+        <v>196</v>
+      </c>
+      <c r="F44" t="s">
+        <v>200</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>